<commit_message>
CL/JD Push, not processes
Key Error
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,46 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melanieruiz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farerilab/Documents/GitHub/Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2301E873-87F4-5048-952E-5F5A255FE4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB33835F-7736-DA4C-BF4C-E0EEB22DEDB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="29480" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="3160" windowWidth="30860" windowHeight="18020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
-    <sheet name="pilotcompletedparticipantlist_o" sheetId="2" r:id="rId3"/>
+    <sheet name="pilotcompletedparticipantlist_o" sheetId="2" r:id="rId1"/>
+    <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId3"/>
     <sheet name="totalparticipantlist_online" sheetId="3" r:id="rId4"/>
     <sheet name="completedparticipantlist_online" sheetId="4" r:id="rId5"/>
     <sheet name="totalparticipantlist_inperson" sheetId="5" r:id="rId6"/>
     <sheet name="completedparticipantlist_inpers" sheetId="6" r:id="rId7"/>
     <sheet name="combined_completedparticipantli" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="90">
   <si>
     <t>sub_id</t>
   </si>
@@ -216,9 +203,6 @@
     <t>SG CL</t>
   </si>
   <si>
-    <t>SjG CL</t>
-  </si>
-  <si>
     <t>R_28Bb6hdQifdwUe3</t>
   </si>
   <si>
@@ -262,6 +246,58 @@
   </si>
   <si>
     <t>5ad2c8334d061300011b1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCS responses to items 1-6 were the same - thoughts? Also did not answer SRQ item 2
+</t>
+  </si>
+  <si>
+    <t>ERQ_16-19 same; AQ_8-12 same</t>
+  </si>
+  <si>
+    <t>AQ_11-20 same; AQ_2-6 same; percieved stress all are same except item 3</t>
+  </si>
+  <si>
+    <t>R_2wyvCnmrBb5A2Us</t>
+  </si>
+  <si>
+    <t>R_2CD10Jlc9GaVYwm</t>
+  </si>
+  <si>
+    <t>R_1llYplkXFJbis2f</t>
+  </si>
+  <si>
+    <t>R_240keg0XIv1Apbh</t>
+  </si>
+  <si>
+    <t>R_Wj1AqUFRO5TzLJD</t>
+  </si>
+  <si>
+    <t>R_xg3XTfbdkPY00Uh</t>
+  </si>
+  <si>
+    <t>SJG CL</t>
+  </si>
+  <si>
+    <t>R_C7DzUG7F5c59TdT</t>
+  </si>
+  <si>
+    <t>R_3jTcFaoXdGyJII6</t>
+  </si>
+  <si>
+    <t>R_1kH5pc9TioLBroe</t>
+  </si>
+  <si>
+    <t>R_2xA9wnR30xhb9aV</t>
+  </si>
+  <si>
+    <t>R_1C3J1A2DE2CFCSm</t>
+  </si>
+  <si>
+    <t>R_3dX5YSGyHAGiLIA</t>
+  </si>
+  <si>
+    <t>RSQ_4a-6a same responses; SCS_1-6 all the same; SRQ_18-23 all the same… photo 30 is a llittle sus</t>
   </si>
 </sst>
 </file>
@@ -335,7 +371,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -375,8 +411,16 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,17 +635,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("FILTER(pilottotalparticipant_list!A:A,pilottotalparticipant_list!I:I = ""y"")"),"R_1QfKCII0MPcPQEB")</f>
+        <v>R_1QfKCII0MPcPQEB</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"R_3jZ4uVvlcxoHLxa")</f>
+        <v>R_3jZ4uVvlcxoHLxa</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"R_1NrJNgK6q4hb04o")</f>
+        <v>R_1NrJNgK6q4hb04o</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -696,7 +782,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1">
         <f>COUNTA(B2:B999)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P2" s="1">
         <f>COUNTIF(N2:N999, "y")</f>
@@ -996,13 +1082,13 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>46</v>
@@ -1017,13 +1103,13 @@
         <v>11</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L13">
         <v>3</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1031,10 +1117,10 @@
         <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
@@ -1049,7 +1135,7 @@
         <v>11</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L14">
         <v>3</v>
@@ -1060,10 +1146,10 @@
         <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
         <v>48</v>
@@ -1078,7 +1164,7 @@
         <v>11</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L15">
         <v>3</v>
@@ -1089,10 +1175,10 @@
         <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
         <v>45</v>
@@ -1107,66 +1193,259 @@
         <v>11</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E17" s="14" t="s">
+    <row r="17" spans="1:13" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="18">
+        <v>44967</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="16">
+        <v>3</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F18" s="22">
         <v>44967</v>
       </c>
-    </row>
-    <row r="18" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E18" s="14" t="s">
+      <c r="G18" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F19" s="22">
         <v>44967</v>
       </c>
-    </row>
-    <row r="19" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E19" s="14" t="s">
+      <c r="G19" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F20" s="22">
         <v>44967</v>
       </c>
-    </row>
-    <row r="20" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E20" s="14" t="s">
+      <c r="G20" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F21" s="22">
         <v>44967</v>
       </c>
-    </row>
-    <row r="21" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E21" s="14" t="s">
+      <c r="G21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F22" s="22">
         <v>44967</v>
       </c>
-    </row>
-    <row r="22" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E22" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="15">
-        <v>44967</v>
-      </c>
+      <c r="G22" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C54368-7267-714C-B261-8D4D6164F801}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1174,48 +1453,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("FILTER(pilottotalparticipant_list!A:A,pilottotalparticipant_list!I:I = ""y"")"),"R_1QfKCII0MPcPQEB")</f>
-        <v>R_1QfKCII0MPcPQEB</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"R_3jZ4uVvlcxoHLxa")</f>
-        <v>R_3jZ4uVvlcxoHLxa</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"R_1NrJNgK6q4hb04o")</f>
-        <v>R_1NrJNgK6q4hb04o</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
JD - Updated Scoring Scripts
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordansiegel/Documents/GitHub/Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFAC27F-3616-B642-BE44-AB490222B7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31681C4-9CE5-A542-8DD3-95AC3DEB305C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34180" yWindow="420" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="91">
   <si>
     <t>qualtrics_selfreport</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>no task data</t>
   </si>
 </sst>
 </file>
@@ -639,7 +642,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1174,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="L17" s="14">
         <v>3</v>

</xml_diff>

<commit_message>
16 participants from 6/5 -- MR
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melanieruiz/Desktop/Rejection_Choice-main 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melanieruiz/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69E3645-5FA1-FE4D-9289-4A2494E5CBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82245C38-7AAE-0849-B665-30B47338628C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="24320" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="760" windowWidth="16300" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="339">
   <si>
     <t>pavlovia_task</t>
   </si>
@@ -1000,6 +1000,57 @@
   </si>
   <si>
     <t>need to contact for 3 new photos of self; only uploaded 2 pics of self</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missed 11 trials </t>
+  </si>
+  <si>
+    <t>60ff1a1450c5e5c8fe6922d1</t>
+  </si>
+  <si>
+    <t>5fd18d125e1f92195b1717bc</t>
+  </si>
+  <si>
+    <t>61006f43a84b82fb439d7cba</t>
+  </si>
+  <si>
+    <t>6129cc7a565c9c03752802fa</t>
+  </si>
+  <si>
+    <t>62f13dc95cf68f5d1182f495</t>
+  </si>
+  <si>
+    <t>595727bd7c76640001aa8f6e</t>
+  </si>
+  <si>
+    <t>62a1ed3d1357f3e033ae44f9</t>
+  </si>
+  <si>
+    <t>63d5e3bf4a739d1158b9ce64</t>
+  </si>
+  <si>
+    <t>612e6569f68929afb886fb5c</t>
+  </si>
+  <si>
+    <t>615a084387075364a7462335</t>
+  </si>
+  <si>
+    <t>61084dbab48ab21fce452554</t>
+  </si>
+  <si>
+    <t>605e52035e8254058df590fa</t>
+  </si>
+  <si>
+    <t>610745dee13497549c9d6fba</t>
+  </si>
+  <si>
+    <t>602c1f715e466a4985a5776f</t>
+  </si>
+  <si>
+    <t>5d8e64ab4e055600157a3d90</t>
+  </si>
+  <si>
+    <t>61002b174a64f106fb46f6a0</t>
   </si>
 </sst>
 </file>
@@ -1095,23 +1146,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1124,6 +1166,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1414,13 +1469,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V92"/>
+  <dimension ref="A1:V103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K84" sqref="K84"/>
+      <selection pane="bottomRight" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1428,15 +1483,14 @@
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="8" width="25.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.83203125" customWidth="1"/>
-    <col min="12" max="14" width="25.5" customWidth="1"/>
-    <col min="15" max="15" width="25.6640625" customWidth="1"/>
-    <col min="16" max="16" width="19.83203125" customWidth="1"/>
-    <col min="17" max="17" width="23" customWidth="1"/>
+    <col min="6" max="8" width="25.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" style="20" hidden="1" customWidth="1"/>
+    <col min="12" max="14" width="25.5" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="25.6640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="25.83203125" customWidth="1"/>
     <col min="19" max="19" width="15.83203125" customWidth="1"/>
   </cols>
@@ -1472,7 +1526,7 @@
       <c r="J1" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="17" t="s">
         <v>31</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -1493,7 +1547,7 @@
       <c r="Q1" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>50</v>
       </c>
       <c r="S1" s="3" t="s">
@@ -1510,15 +1564,15 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1"/>
@@ -1534,13 +1588,12 @@
       <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="7"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1">
         <f>COUNTA(B2:B998)</f>
@@ -1556,18 +1609,18 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="6"/>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1580,31 +1633,31 @@
       <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="18" t="s">
         <v>87</v>
       </c>
       <c r="P3" s="1"/>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="10" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1617,26 +1670,25 @@
       <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="18" t="s">
         <v>87</v>
       </c>
       <c r="P4" s="1"/>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="7"/>
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -1645,20 +1697,19 @@
       <c r="J5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -1667,22 +1718,21 @@
       <c r="J6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="7"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -1691,37 +1741,36 @@
       <c r="J7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:22" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>44873</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <v>44872</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="G8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1730,7 +1779,7 @@
       <c r="J8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="18" t="s">
         <v>9</v>
       </c>
       <c r="L8">
@@ -1739,39 +1788,39 @@
       <c r="N8">
         <v>1</v>
       </c>
-      <c r="P8" s="12">
+      <c r="P8" s="9">
         <v>2</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="R8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
         <v>44873</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>44872</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="G9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -1780,14 +1829,14 @@
       <c r="J9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="5">
-        <v>1</v>
-      </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5">
+      <c r="K9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4">
         <v>1</v>
       </c>
       <c r="P9">
@@ -1796,16 +1845,15 @@
       <c r="Q9">
         <v>0</v>
       </c>
-      <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>44881</v>
       </c>
       <c r="D10" t="s">
@@ -1814,7 +1862,7 @@
       <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>44879</v>
       </c>
       <c r="G10" t="s">
@@ -1829,14 +1877,14 @@
       <c r="J10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" s="5">
-        <v>1</v>
-      </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5">
+      <c r="K10" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="4">
+        <v>1</v>
+      </c>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4">
         <v>1</v>
       </c>
       <c r="P10">
@@ -1847,13 +1895,13 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>44881</v>
       </c>
       <c r="D11" t="s">
@@ -1862,13 +1910,13 @@
       <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>44879</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1877,14 +1925,14 @@
       <c r="J11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="5">
-        <v>1</v>
-      </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5">
+      <c r="K11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4">
         <v>1</v>
       </c>
       <c r="P11">
@@ -1895,13 +1943,13 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>44881</v>
       </c>
       <c r="D12" t="s">
@@ -1910,13 +1958,13 @@
       <c r="E12" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>44879</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="5" t="s">
+      <c r="G12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -1925,14 +1973,14 @@
       <c r="J12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="5">
-        <v>1</v>
-      </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5">
+      <c r="K12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1</v>
+      </c>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4">
         <v>1</v>
       </c>
       <c r="P12">
@@ -1943,13 +1991,13 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="8">
         <v>44958</v>
       </c>
       <c r="D13" t="s">
@@ -1958,13 +2006,13 @@
       <c r="E13" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <v>44958</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1973,14 +2021,14 @@
       <c r="J13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="5">
-        <v>1</v>
-      </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5">
+      <c r="K13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="4">
+        <v>1</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4">
         <v>1</v>
       </c>
       <c r="Q13">
@@ -1988,7 +2036,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B14" t="s">
@@ -2000,29 +2048,29 @@
       <c r="E14" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8">
         <v>44959</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="5" t="s">
+      <c r="G14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L14" s="5">
-        <v>1</v>
-      </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5">
+      <c r="K14" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4">
         <v>1</v>
       </c>
       <c r="P14">
@@ -2031,12 +2079,12 @@
       <c r="Q14">
         <v>0</v>
       </c>
-      <c r="R14" s="5" t="s">
+      <c r="R14" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B15" t="s">
@@ -2048,13 +2096,13 @@
       <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="8">
         <v>44959</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="5" t="s">
+      <c r="G15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -2063,14 +2111,14 @@
       <c r="J15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L15" s="5">
-        <v>1</v>
-      </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5">
+      <c r="K15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4">
         <v>1</v>
       </c>
       <c r="P15">
@@ -2081,7 +2129,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B16" t="s">
@@ -2093,13 +2141,13 @@
       <c r="E16" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="8">
         <v>44959</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="G16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -2108,14 +2156,14 @@
       <c r="J16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L16" s="5">
-        <v>1</v>
-      </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5">
+      <c r="K16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4">
         <v>1</v>
       </c>
       <c r="P16">
@@ -2126,7 +2174,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
@@ -2138,13 +2186,13 @@
       <c r="E17" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>44959</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="5" t="s">
+      <c r="G17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -2153,14 +2201,14 @@
       <c r="J17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17" s="5">
-        <v>1</v>
-      </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5">
+      <c r="K17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4">
         <v>0</v>
       </c>
       <c r="P17">
@@ -2171,7 +2219,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B18" t="s">
@@ -2180,16 +2228,16 @@
       <c r="D18" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="8">
         <v>44967</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="G18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -2198,12 +2246,12 @@
       <c r="J18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="5">
-        <v>0</v>
-      </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5">
+      <c r="K18" s="18"/>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4">
         <v>1</v>
       </c>
       <c r="P18">
@@ -2212,12 +2260,12 @@
       <c r="Q18">
         <v>0</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="R18" s="4" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B19" t="s">
@@ -2226,16 +2274,16 @@
       <c r="D19" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="8">
         <v>44967</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="5" t="s">
+      <c r="G19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -2244,14 +2292,14 @@
       <c r="J19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19" s="5">
-        <v>1</v>
-      </c>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5">
+      <c r="K19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="4">
+        <v>1</v>
+      </c>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4">
         <v>1</v>
       </c>
       <c r="P19">
@@ -2260,12 +2308,12 @@
       <c r="Q19">
         <v>0</v>
       </c>
-      <c r="R19" s="7" t="s">
+      <c r="R19" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B20" t="s">
@@ -2274,16 +2322,16 @@
       <c r="D20" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="8">
         <v>44967</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -2292,14 +2340,14 @@
       <c r="J20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L20" s="5">
-        <v>1</v>
-      </c>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5">
+      <c r="K20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1</v>
+      </c>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4">
         <v>1</v>
       </c>
       <c r="P20">
@@ -2310,7 +2358,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B21" t="s">
@@ -2319,16 +2367,16 @@
       <c r="D21" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="8">
         <v>44967</v>
       </c>
       <c r="G21" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -2337,14 +2385,14 @@
       <c r="J21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="5">
-        <v>1</v>
-      </c>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5">
+      <c r="K21" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="4">
+        <v>1</v>
+      </c>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4">
         <v>1</v>
       </c>
       <c r="P21">
@@ -2358,7 +2406,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B22" t="s">
@@ -2367,16 +2415,16 @@
       <c r="D22" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="8">
         <v>44967</v>
       </c>
       <c r="G22" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -2385,19 +2433,19 @@
       <c r="J22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L22" s="5">
-        <v>1</v>
-      </c>
-      <c r="M22" s="5" t="s">
+      <c r="K22" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" s="4">
+        <v>1</v>
+      </c>
+      <c r="M22" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="N22" s="5">
-        <v>0</v>
-      </c>
-      <c r="O22" s="5"/>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
+      <c r="O22" s="4"/>
       <c r="P22">
         <v>3</v>
       </c>
@@ -2409,7 +2457,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B23" t="s">
@@ -2418,16 +2466,16 @@
       <c r="D23" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="8">
         <v>44967</v>
       </c>
       <c r="G23" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -2436,14 +2484,14 @@
       <c r="J23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L23" s="5">
-        <v>1</v>
-      </c>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5">
+      <c r="K23" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="4">
+        <v>1</v>
+      </c>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4">
         <v>1</v>
       </c>
       <c r="P23">
@@ -2454,28 +2502,28 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B24" t="s">
         <v>146</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="8">
         <v>44977</v>
       </c>
       <c r="D24" t="s">
         <v>112</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="6">
         <v>44977</v>
       </c>
       <c r="G24" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -2484,14 +2532,14 @@
       <c r="J24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L24" s="5">
-        <v>1</v>
-      </c>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5">
+      <c r="K24" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1</v>
+      </c>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4">
         <v>1</v>
       </c>
       <c r="Q24">
@@ -2502,28 +2550,28 @@
       </c>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B25" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="8">
         <v>44977</v>
       </c>
       <c r="D25" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="6">
         <v>44977</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -2532,14 +2580,14 @@
       <c r="J25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L25" s="5">
-        <v>1</v>
-      </c>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5">
+      <c r="K25" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1</v>
+      </c>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4">
         <v>1</v>
       </c>
       <c r="Q25">
@@ -2547,28 +2595,28 @@
       </c>
     </row>
     <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B26" t="s">
         <v>130</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="8">
         <v>44977</v>
       </c>
       <c r="D26" t="s">
         <v>114</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="6">
         <v>44977</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -2577,14 +2625,14 @@
       <c r="J26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L26" s="5">
-        <v>1</v>
-      </c>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5">
+      <c r="K26" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L26" s="4">
+        <v>1</v>
+      </c>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4">
         <v>1</v>
       </c>
       <c r="Q26">
@@ -2595,28 +2643,28 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B27" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="8">
         <v>44977</v>
       </c>
       <c r="D27" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="6">
         <v>44977</v>
       </c>
       <c r="G27" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -2625,62 +2673,62 @@
       <c r="J27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L27" s="5">
-        <v>1</v>
-      </c>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5">
+      <c r="K27" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L27" s="4">
+        <v>1</v>
+      </c>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4">
         <v>1</v>
       </c>
       <c r="Q27">
         <v>0</v>
       </c>
-      <c r="R27" s="5" t="s">
+      <c r="R27" s="4" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B28" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="8">
         <v>44977</v>
       </c>
       <c r="D28" t="s">
         <v>116</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="6">
         <v>44977</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="L28" s="5">
-        <v>0</v>
-      </c>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5">
+      <c r="L28" s="4">
+        <v>0</v>
+      </c>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4">
         <v>0</v>
       </c>
       <c r="Q28">
@@ -2691,44 +2739,44 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B29" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="8">
         <v>44977</v>
       </c>
       <c r="D29" t="s">
         <v>117</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="6">
         <v>44977</v>
       </c>
       <c r="G29" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="K29" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="L29" s="5">
-        <v>0</v>
-      </c>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5">
+      <c r="L29" s="4">
+        <v>0</v>
+      </c>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4">
         <v>0</v>
       </c>
       <c r="Q29">
@@ -2739,44 +2787,44 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B30" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="8">
         <v>44977</v>
       </c>
       <c r="D30" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="6">
         <v>44977</v>
       </c>
       <c r="G30" t="s">
         <v>9</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="I30" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L30" s="5">
-        <v>1</v>
-      </c>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5">
+      <c r="K30" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" s="4">
+        <v>1</v>
+      </c>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4">
         <v>1</v>
       </c>
       <c r="Q30">
@@ -2784,92 +2832,92 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B31" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="8">
         <v>44977</v>
       </c>
       <c r="D31" t="s">
         <v>119</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="6">
         <v>44977</v>
       </c>
       <c r="G31" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31" s="5" t="s">
+      <c r="H31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L31" s="5">
-        <v>1</v>
-      </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5">
+      <c r="K31" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" s="4">
+        <v>1</v>
+      </c>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4">
         <v>1</v>
       </c>
       <c r="Q31">
         <v>0</v>
       </c>
-      <c r="R31" s="5" t="s">
+      <c r="R31" s="4" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B32" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="8">
         <v>44977</v>
       </c>
       <c r="D32" t="s">
         <v>120</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="6">
         <v>44977</v>
       </c>
       <c r="G32" t="s">
         <v>9</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="K32" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="L32" s="5">
-        <v>0</v>
-      </c>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5">
+      <c r="L32" s="4">
+        <v>0</v>
+      </c>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4">
         <v>0</v>
       </c>
       <c r="Q32">
@@ -2877,44 +2925,44 @@
       </c>
     </row>
     <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B33" t="s">
         <v>137</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="8">
         <v>44977</v>
       </c>
       <c r="D33" t="s">
         <v>121</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="6">
         <v>44977</v>
       </c>
       <c r="G33" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I33" s="5" t="s">
+      <c r="H33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L33" s="5">
-        <v>1</v>
-      </c>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5">
+      <c r="K33" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L33" s="4">
+        <v>1</v>
+      </c>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4">
         <v>1</v>
       </c>
       <c r="Q33">
@@ -2922,140 +2970,140 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B34" t="s">
         <v>138</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="8">
         <v>44977</v>
       </c>
       <c r="D34" t="s">
         <v>122</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="6">
         <v>44977</v>
       </c>
       <c r="G34" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I34" s="5" t="s">
+      <c r="H34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K34" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L34" s="5">
-        <v>1</v>
-      </c>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5">
+      <c r="K34" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L34" s="4">
+        <v>1</v>
+      </c>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4">
         <v>1</v>
       </c>
       <c r="Q34">
         <v>0</v>
       </c>
-      <c r="R34" s="5" t="s">
+      <c r="R34" s="4" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B35" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="8">
         <v>44977</v>
       </c>
       <c r="D35" t="s">
         <v>123</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="6">
         <v>44977</v>
       </c>
       <c r="G35" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="H35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="K35" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="L35" s="5">
-        <v>0</v>
-      </c>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5">
+      <c r="L35" s="4">
+        <v>0</v>
+      </c>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4">
         <v>0</v>
       </c>
       <c r="Q35">
         <v>0</v>
       </c>
-      <c r="R35" s="5" t="s">
+      <c r="R35" s="4" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B36" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="8">
         <v>44977</v>
       </c>
       <c r="D36" t="s">
         <v>111</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="6">
         <v>44977</v>
       </c>
       <c r="G36" t="s">
         <v>9</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="I36" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="K36" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="L36" s="5">
-        <v>0</v>
-      </c>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5">
+      <c r="L36" s="4">
+        <v>0</v>
+      </c>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4">
         <v>0</v>
       </c>
       <c r="Q36">
@@ -3066,92 +3114,92 @@
       </c>
     </row>
     <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B37" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="8">
         <v>44977</v>
       </c>
       <c r="D37" t="s">
         <v>124</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="6">
         <v>44977</v>
       </c>
       <c r="G37" t="s">
         <v>9</v>
       </c>
-      <c r="H37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I37" s="5" t="s">
+      <c r="H37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L37" s="5">
-        <v>1</v>
-      </c>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5">
+      <c r="K37" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" s="4">
+        <v>1</v>
+      </c>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4">
         <v>1</v>
       </c>
       <c r="Q37">
         <v>0</v>
       </c>
-      <c r="R37" s="5" t="s">
+      <c r="R37" s="4" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B38" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="8">
         <v>44977</v>
       </c>
       <c r="D38" t="s">
         <v>125</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="6">
         <v>44977</v>
       </c>
       <c r="G38" t="s">
         <v>9</v>
       </c>
-      <c r="H38" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I38" s="5" t="s">
+      <c r="H38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K38" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L38" s="5">
-        <v>1</v>
-      </c>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5">
+      <c r="K38" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L38" s="4">
+        <v>1</v>
+      </c>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4">
         <v>1</v>
       </c>
       <c r="Q38">
@@ -3159,44 +3207,44 @@
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B39" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="8">
         <v>44977</v>
       </c>
       <c r="D39" t="s">
         <v>126</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="6">
         <v>44977</v>
       </c>
       <c r="G39" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="H39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="K39" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="L39" s="5">
-        <v>0</v>
-      </c>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5">
+      <c r="L39" s="4">
+        <v>0</v>
+      </c>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4">
         <v>0</v>
       </c>
       <c r="Q39">
@@ -3204,92 +3252,92 @@
       </c>
     </row>
     <row r="40" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B40" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="8">
         <v>44977</v>
       </c>
       <c r="D40" t="s">
         <v>127</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F40" s="6">
         <v>44977</v>
       </c>
       <c r="G40" t="s">
         <v>9</v>
       </c>
-      <c r="H40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I40" s="5" t="s">
+      <c r="H40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L40" s="5">
-        <v>1</v>
-      </c>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5">
+      <c r="K40" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" s="4">
+        <v>1</v>
+      </c>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4">
         <v>1</v>
       </c>
       <c r="Q40">
         <v>0</v>
       </c>
-      <c r="R40" s="5" t="s">
+      <c r="R40" s="4" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B41" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="8">
         <v>44977</v>
       </c>
       <c r="D41" t="s">
         <v>128</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="6">
         <v>44977</v>
       </c>
       <c r="G41" t="s">
         <v>9</v>
       </c>
-      <c r="H41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I41" s="5" t="s">
+      <c r="H41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L41" s="5">
-        <v>1</v>
-      </c>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5">
+      <c r="K41" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L41" s="4">
+        <v>1</v>
+      </c>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4">
         <v>1</v>
       </c>
       <c r="Q41">
@@ -3300,80 +3348,80 @@
       </c>
     </row>
     <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B42" t="s">
         <v>195</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="8">
         <v>44994</v>
       </c>
       <c r="D42" t="s">
         <v>177</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="F42" s="16">
+      <c r="F42" s="13">
         <v>44993</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L42" s="5">
-        <v>1</v>
-      </c>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5">
-        <v>1</v>
-      </c>
-      <c r="P42" s="5" t="s">
+      <c r="K42" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" s="4">
+        <v>1</v>
+      </c>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4">
+        <v>1</v>
+      </c>
+      <c r="P42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q42">
         <v>1</v>
       </c>
-      <c r="R42" s="5" t="s">
+      <c r="R42" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B43" t="s">
         <v>196</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="8">
         <v>44994</v>
       </c>
       <c r="D43" t="s">
         <v>178</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="F43" s="16">
+      <c r="F43" s="13">
         <v>44993</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K43" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L43" s="5">
-        <v>1</v>
-      </c>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5">
-        <v>1</v>
-      </c>
-      <c r="P43" s="5" t="s">
+      <c r="K43" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L43" s="4">
+        <v>1</v>
+      </c>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4">
+        <v>1</v>
+      </c>
+      <c r="P43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q43">
@@ -3381,80 +3429,80 @@
       </c>
     </row>
     <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B44" t="s">
         <v>197</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="8">
         <v>44994</v>
       </c>
       <c r="D44" t="s">
         <v>179</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="F44" s="16">
+      <c r="F44" s="13">
         <v>44993</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K44" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L44" s="5">
-        <v>1</v>
-      </c>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5">
-        <v>1</v>
-      </c>
-      <c r="P44" s="5" t="s">
+      <c r="K44" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L44" s="4">
+        <v>1</v>
+      </c>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4">
+        <v>1</v>
+      </c>
+      <c r="P44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q44">
         <v>1</v>
       </c>
-      <c r="R44" s="5" t="s">
+      <c r="R44" s="4" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B45" t="s">
         <v>198</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="8">
         <v>44994</v>
       </c>
       <c r="D45" t="s">
         <v>180</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="F45" s="16">
+      <c r="F45" s="13">
         <v>44993</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K45" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L45" s="5">
-        <v>1</v>
-      </c>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5">
-        <v>1</v>
-      </c>
-      <c r="P45" s="5" t="s">
+      <c r="K45" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1</v>
+      </c>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4">
+        <v>1</v>
+      </c>
+      <c r="P45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q45">
@@ -3462,164 +3510,164 @@
       </c>
     </row>
     <row r="46" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B46" t="s">
         <v>199</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C46" s="8">
         <v>44994</v>
       </c>
       <c r="D46" t="s">
         <v>181</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F46" s="16">
+      <c r="F46" s="13">
         <v>44993</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K46" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L46" s="5">
-        <v>1</v>
-      </c>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5">
-        <v>1</v>
-      </c>
-      <c r="P46" s="5" t="s">
+      <c r="K46" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L46" s="4">
+        <v>1</v>
+      </c>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4">
+        <v>1</v>
+      </c>
+      <c r="P46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q46">
         <v>1</v>
       </c>
-      <c r="R46" s="5" t="s">
+      <c r="R46" s="4" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B47" t="s">
         <v>200</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C47" s="8">
         <v>44994</v>
       </c>
       <c r="D47" t="s">
         <v>182</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="F47" s="16">
+      <c r="F47" s="13">
         <v>44993</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L47" s="5">
-        <v>1</v>
-      </c>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5">
-        <v>1</v>
-      </c>
-      <c r="P47" s="5" t="s">
+      <c r="K47" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" s="4">
+        <v>1</v>
+      </c>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4">
+        <v>1</v>
+      </c>
+      <c r="P47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q47">
         <v>1</v>
       </c>
-      <c r="R47" s="5" t="s">
+      <c r="R47" s="4" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B48" t="s">
         <v>201</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C48" s="8">
         <v>44994</v>
       </c>
       <c r="D48" t="s">
         <v>183</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="F48" s="16">
+      <c r="F48" s="13">
         <v>44993</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K48" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L48" s="5">
-        <v>1</v>
-      </c>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5">
-        <v>1</v>
-      </c>
-      <c r="P48" s="5" t="s">
+      <c r="K48" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L48" s="4">
+        <v>1</v>
+      </c>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4">
+        <v>1</v>
+      </c>
+      <c r="P48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q48">
         <v>1</v>
       </c>
-      <c r="R48" s="5" t="s">
+      <c r="R48" s="4" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B49" t="s">
         <v>202</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="8">
         <v>44994</v>
       </c>
       <c r="D49" t="s">
         <v>184</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="E49" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="16">
+      <c r="F49" s="13">
         <v>44993</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K49" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L49" s="5">
-        <v>1</v>
-      </c>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5">
-        <v>1</v>
-      </c>
-      <c r="P49" s="5" t="s">
+      <c r="K49" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L49" s="4">
+        <v>1</v>
+      </c>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4">
+        <v>1</v>
+      </c>
+      <c r="P49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q49">
@@ -3627,38 +3675,38 @@
       </c>
     </row>
     <row r="50" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B50" t="s">
         <v>203</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="8">
         <v>44994</v>
       </c>
       <c r="D50" t="s">
         <v>185</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="F50" s="16">
+      <c r="F50" s="13">
         <v>44993</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L50" s="5">
-        <v>1</v>
-      </c>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5">
-        <v>1</v>
-      </c>
-      <c r="P50" s="5" t="s">
+      <c r="K50" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L50" s="4">
+        <v>1</v>
+      </c>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4">
+        <v>1</v>
+      </c>
+      <c r="P50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q50">
@@ -3666,38 +3714,38 @@
       </c>
     </row>
     <row r="51" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B51" t="s">
         <v>204</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="8">
         <v>44994</v>
       </c>
       <c r="D51" t="s">
         <v>186</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="F51" s="16">
+      <c r="F51" s="13">
         <v>44993</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L51" s="5">
-        <v>1</v>
-      </c>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5">
-        <v>1</v>
-      </c>
-      <c r="P51" s="5" t="s">
+      <c r="K51" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L51" s="4">
+        <v>1</v>
+      </c>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4">
+        <v>1</v>
+      </c>
+      <c r="P51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q51">
@@ -3705,38 +3753,38 @@
       </c>
     </row>
     <row r="52" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B52" t="s">
         <v>205</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="8">
         <v>44994</v>
       </c>
       <c r="D52" t="s">
         <v>187</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="F52" s="11">
+      <c r="F52" s="8">
         <v>44993</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K52" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L52" s="5">
-        <v>1</v>
-      </c>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5">
-        <v>1</v>
-      </c>
-      <c r="P52" s="5" t="s">
+      <c r="K52" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L52" s="4">
+        <v>1</v>
+      </c>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4">
+        <v>1</v>
+      </c>
+      <c r="P52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q52">
@@ -3744,38 +3792,38 @@
       </c>
     </row>
     <row r="53" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B53" t="s">
         <v>206</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="8">
         <v>44994</v>
       </c>
       <c r="D53" t="s">
         <v>188</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="F53" s="11">
+      <c r="F53" s="8">
         <v>44993</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K53" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L53" s="5">
-        <v>1</v>
-      </c>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5">
-        <v>1</v>
-      </c>
-      <c r="P53" s="5" t="s">
+      <c r="K53" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L53" s="4">
+        <v>1</v>
+      </c>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4">
+        <v>1</v>
+      </c>
+      <c r="P53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q53">
@@ -3786,80 +3834,80 @@
       </c>
     </row>
     <row r="54" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B54" t="s">
         <v>207</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="8">
         <v>44994</v>
       </c>
       <c r="D54" t="s">
         <v>189</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="E54" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="F54" s="11">
+      <c r="F54" s="8">
         <v>44993</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K54" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L54" s="5">
-        <v>1</v>
-      </c>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5">
-        <v>1</v>
-      </c>
-      <c r="P54" s="5" t="s">
+      <c r="K54" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L54" s="4">
+        <v>1</v>
+      </c>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4">
+        <v>1</v>
+      </c>
+      <c r="P54" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q54">
         <v>1</v>
       </c>
-      <c r="R54" s="5" t="s">
+      <c r="R54" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B55" t="s">
         <v>208</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="8">
         <v>44994</v>
       </c>
       <c r="D55" t="s">
         <v>191</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F55" s="11">
+      <c r="F55" s="8">
         <v>44993</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K55" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L55" s="5">
-        <v>1</v>
-      </c>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5">
-        <v>1</v>
-      </c>
-      <c r="P55" s="5" t="s">
+      <c r="K55" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L55" s="4">
+        <v>1</v>
+      </c>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4">
+        <v>1</v>
+      </c>
+      <c r="P55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q55">
@@ -3867,38 +3915,38 @@
       </c>
     </row>
     <row r="56" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B56" t="s">
         <v>209</v>
       </c>
-      <c r="C56" s="11">
+      <c r="C56" s="8">
         <v>44994</v>
       </c>
       <c r="D56" t="s">
         <v>192</v>
       </c>
-      <c r="E56" s="14" t="s">
+      <c r="E56" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="F56" s="11">
+      <c r="F56" s="8">
         <v>44993</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K56" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L56" s="5">
-        <v>1</v>
-      </c>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5">
-        <v>1</v>
-      </c>
-      <c r="P56" s="5" t="s">
+      <c r="K56" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L56" s="4">
+        <v>1</v>
+      </c>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4">
+        <v>1</v>
+      </c>
+      <c r="P56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q56">
@@ -3906,38 +3954,38 @@
       </c>
     </row>
     <row r="57" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B57" t="s">
         <v>210</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="8">
         <v>44994</v>
       </c>
       <c r="D57" t="s">
         <v>193</v>
       </c>
-      <c r="E57" s="14" t="s">
+      <c r="E57" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="F57" s="11">
+      <c r="F57" s="8">
         <v>44993</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K57" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L57" s="5">
-        <v>1</v>
-      </c>
-      <c r="M57" s="5"/>
-      <c r="N57" s="5">
-        <v>1</v>
-      </c>
-      <c r="P57" s="5" t="s">
+      <c r="K57" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L57" s="4">
+        <v>1</v>
+      </c>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4">
+        <v>1</v>
+      </c>
+      <c r="P57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q57">
@@ -3945,80 +3993,80 @@
       </c>
     </row>
     <row r="58" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B58" t="s">
         <v>211</v>
       </c>
-      <c r="C58" s="11">
+      <c r="C58" s="8">
         <v>44994</v>
       </c>
       <c r="D58" t="s">
         <v>194</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E58" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="F58" s="11">
+      <c r="F58" s="8">
         <v>44993</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K58" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L58" s="5">
-        <v>1</v>
-      </c>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5">
-        <v>1</v>
-      </c>
-      <c r="P58" s="5" t="s">
+      <c r="K58" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L58" s="4">
+        <v>1</v>
+      </c>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4">
+        <v>1</v>
+      </c>
+      <c r="P58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q58">
         <v>1</v>
       </c>
-      <c r="R58" s="5" t="s">
+      <c r="R58" s="4" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B59" t="s">
         <v>241</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="8">
         <v>45005</v>
       </c>
       <c r="D59" t="s">
         <v>228</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="E59" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="F59" s="11">
+      <c r="F59" s="8">
         <v>45004</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="I59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K59" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L59" s="5">
-        <v>1</v>
-      </c>
-      <c r="M59" s="5"/>
-      <c r="N59" s="5">
+      <c r="K59" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L59" s="4">
+        <v>1</v>
+      </c>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4">
         <v>1</v>
       </c>
       <c r="Q59">
@@ -4026,38 +4074,38 @@
       </c>
     </row>
     <row r="60" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B60" t="s">
         <v>237</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="8">
         <v>45005</v>
       </c>
       <c r="D60" t="s">
         <v>229</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="E60" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="F60" s="11">
+      <c r="F60" s="8">
         <v>37334</v>
       </c>
-      <c r="I60" s="5" t="s">
+      <c r="I60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K60" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L60" s="5">
-        <v>1</v>
-      </c>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5">
+      <c r="K60" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L60" s="4">
+        <v>1</v>
+      </c>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4">
         <v>1</v>
       </c>
       <c r="Q60">
@@ -4065,38 +4113,38 @@
       </c>
     </row>
     <row r="61" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B61" t="s">
         <v>240</v>
       </c>
-      <c r="C61" s="11">
+      <c r="C61" s="8">
         <v>45005</v>
       </c>
       <c r="D61" t="s">
         <v>230</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="F61" s="11">
+      <c r="F61" s="8">
         <v>37334</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K61" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L61" s="5">
-        <v>1</v>
-      </c>
-      <c r="M61" s="5"/>
-      <c r="N61" s="5">
+      <c r="K61" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L61" s="4">
+        <v>1</v>
+      </c>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4">
         <v>1</v>
       </c>
       <c r="Q61">
@@ -4104,38 +4152,38 @@
       </c>
     </row>
     <row r="62" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B62" t="s">
         <v>239</v>
       </c>
-      <c r="C62" s="11">
+      <c r="C62" s="8">
         <v>45005</v>
       </c>
       <c r="D62" t="s">
         <v>231</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="E62" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="F62" s="11">
+      <c r="F62" s="8">
         <v>37334</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="I62" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K62" s="5" t="s">
+      <c r="K62" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="L62" s="5">
-        <v>0</v>
-      </c>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5">
+      <c r="L62" s="4">
+        <v>0</v>
+      </c>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4">
         <v>0</v>
       </c>
       <c r="Q62">
@@ -4143,69 +4191,69 @@
       </c>
     </row>
     <row r="63" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="5"/>
+      <c r="A63" s="4"/>
       <c r="E63" t="s">
         <v>224</v>
       </c>
-      <c r="F63" s="11">
+      <c r="F63" s="8">
         <v>37334</v>
       </c>
-      <c r="I63" s="5" t="s">
+      <c r="I63" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K63" s="5" t="s">
+      <c r="K63" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="L63" s="5">
-        <v>0</v>
-      </c>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5">
+      <c r="L63" s="4">
+        <v>0</v>
+      </c>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4">
         <v>0</v>
       </c>
       <c r="Q63">
         <v>1</v>
       </c>
-      <c r="R63" s="5" t="s">
+      <c r="R63" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C64" s="11">
+      <c r="C64" s="8">
         <v>45005</v>
       </c>
       <c r="D64" t="s">
         <v>232</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E64" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="F64" s="11">
+      <c r="F64" s="8">
         <v>45005</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="I64" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K64" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L64" s="5">
-        <v>1</v>
-      </c>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5">
+      <c r="K64" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L64" s="4">
+        <v>1</v>
+      </c>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4">
         <v>1</v>
       </c>
       <c r="Q64">
@@ -4213,38 +4261,38 @@
       </c>
     </row>
     <row r="65" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B65" t="s">
         <v>242</v>
       </c>
-      <c r="C65" s="11">
+      <c r="C65" s="8">
         <v>45005</v>
       </c>
       <c r="D65" t="s">
         <v>233</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="F65" s="11">
+      <c r="F65" s="8">
         <v>45005</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="I65" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K65" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L65" s="5">
-        <v>1</v>
-      </c>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5">
+      <c r="K65" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L65" s="4">
+        <v>1</v>
+      </c>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4">
         <v>1</v>
       </c>
       <c r="Q65">
@@ -4252,38 +4300,38 @@
       </c>
     </row>
     <row r="66" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B66" t="s">
         <v>236</v>
       </c>
-      <c r="C66" s="11">
+      <c r="C66" s="8">
         <v>45005</v>
       </c>
       <c r="D66" t="s">
         <v>235</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="E66" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="F66" s="11">
+      <c r="F66" s="8">
         <v>45004</v>
       </c>
-      <c r="I66" s="5" t="s">
+      <c r="I66" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K66" s="5" t="s">
+      <c r="K66" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="L66" s="5">
-        <v>1</v>
-      </c>
-      <c r="M66" s="5"/>
-      <c r="N66" s="5">
+      <c r="L66" s="4">
+        <v>1</v>
+      </c>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4">
         <v>1</v>
       </c>
       <c r="Q66">
@@ -4291,7 +4339,7 @@
       </c>
     </row>
     <row r="67" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B67" t="s">
@@ -4300,27 +4348,27 @@
       <c r="D67" t="s">
         <v>265</v>
       </c>
-      <c r="E67" s="14" t="s">
+      <c r="E67" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F67" s="11">
+      <c r="F67" s="8">
         <v>45014</v>
       </c>
-      <c r="I67" s="5" t="s">
+      <c r="I67" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K67" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P67" s="5" t="s">
+      <c r="K67" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P67" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B68" t="s">
@@ -4329,27 +4377,27 @@
       <c r="D68" t="s">
         <v>266</v>
       </c>
-      <c r="E68" s="14" t="s">
+      <c r="E68" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="F68" s="11">
+      <c r="F68" s="8">
         <v>45014</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="I68" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K68" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P68" s="5" t="s">
+      <c r="K68" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P68" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B69" t="s">
@@ -4358,27 +4406,27 @@
       <c r="D69" t="s">
         <v>267</v>
       </c>
-      <c r="E69" s="14" t="s">
+      <c r="E69" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="F69" s="11">
+      <c r="F69" s="8">
         <v>45014</v>
       </c>
-      <c r="I69" s="5" t="s">
+      <c r="I69" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K69" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P69" s="18" t="s">
+      <c r="K69" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P69" s="15" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B70" t="s">
@@ -4387,27 +4435,27 @@
       <c r="D70" t="s">
         <v>269</v>
       </c>
-      <c r="E70" s="14" t="s">
+      <c r="E70" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="F70" s="11">
+      <c r="F70" s="8">
         <v>45014</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="I70" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K70" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P70" s="5" t="s">
+      <c r="K70" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P70" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B71" t="s">
@@ -4416,27 +4464,27 @@
       <c r="D71" t="s">
         <v>270</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="E71" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="F71" s="11">
+      <c r="F71" s="8">
         <v>45014</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I71" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K71" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P71" s="5" t="s">
+      <c r="K71" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P71" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B72" t="s">
@@ -4445,27 +4493,27 @@
       <c r="D72" t="s">
         <v>271</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="E72" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="F72" s="11">
+      <c r="F72" s="8">
         <v>45014</v>
       </c>
-      <c r="I72" s="5" t="s">
+      <c r="I72" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K72" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P72" s="5" t="s">
+      <c r="K72" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P72" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B73" t="s">
@@ -4474,27 +4522,27 @@
       <c r="D73" t="s">
         <v>272</v>
       </c>
-      <c r="E73" s="14" t="s">
+      <c r="E73" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="F73" s="11">
+      <c r="F73" s="8">
         <v>45014</v>
       </c>
-      <c r="I73" s="5" t="s">
+      <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K73" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P73" s="5" t="s">
+      <c r="K73" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P73" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B74" t="s">
@@ -4503,27 +4551,27 @@
       <c r="D74" t="s">
         <v>273</v>
       </c>
-      <c r="E74" s="14" t="s">
+      <c r="E74" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="F74" s="11">
+      <c r="F74" s="8">
         <v>45014</v>
       </c>
-      <c r="I74" s="5" t="s">
+      <c r="I74" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K74" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P74" s="5" t="s">
+      <c r="K74" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P74" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B75" t="s">
@@ -4532,27 +4580,27 @@
       <c r="D75" t="s">
         <v>274</v>
       </c>
-      <c r="E75" s="14" t="s">
+      <c r="E75" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="F75" s="11">
+      <c r="F75" s="8">
         <v>45014</v>
       </c>
-      <c r="I75" s="5" t="s">
+      <c r="I75" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K75" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P75" s="5" t="s">
+      <c r="K75" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P75" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B76" t="s">
@@ -4561,27 +4609,27 @@
       <c r="D76" t="s">
         <v>275</v>
       </c>
-      <c r="E76" s="14" t="s">
+      <c r="E76" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="F76" s="11">
+      <c r="F76" s="8">
         <v>45014</v>
       </c>
-      <c r="I76" s="5" t="s">
+      <c r="I76" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K76" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P76" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="5" t="s">
+      <c r="K76" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P76" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" ht="14" x14ac:dyDescent="0.15">
+      <c r="A77" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B77" t="s">
@@ -4590,22 +4638,22 @@
       <c r="D77" t="s">
         <v>276</v>
       </c>
-      <c r="E77" s="15" t="s">
+      <c r="E77" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="F77" s="11">
+      <c r="F77" s="8">
         <v>45014</v>
       </c>
-      <c r="I77" s="5" t="s">
+      <c r="I77" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K77" s="5" t="s">
+      <c r="K77" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="P77" s="5" t="s">
+      <c r="P77" s="4" t="s">
         <v>9</v>
       </c>
       <c r="R77" t="s">
@@ -4613,7 +4661,7 @@
       </c>
     </row>
     <row r="78" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B78" t="s">
@@ -4622,27 +4670,27 @@
       <c r="D78" t="s">
         <v>277</v>
       </c>
-      <c r="E78" s="14" t="s">
+      <c r="E78" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="F78" s="11">
+      <c r="F78" s="8">
         <v>45014</v>
       </c>
-      <c r="I78" s="5" t="s">
+      <c r="I78" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K78" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P78" s="5" t="s">
+      <c r="K78" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="P78" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B79" t="s">
@@ -4651,10 +4699,10 @@
       <c r="D79" t="s">
         <v>278</v>
       </c>
-      <c r="E79" s="14" t="s">
+      <c r="E79" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="F79" s="11">
+      <c r="F79" s="8">
         <v>45014</v>
       </c>
       <c r="I79" t="s">
@@ -4663,18 +4711,18 @@
       <c r="J79" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K79" s="5" t="s">
+      <c r="K79" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="P79" s="5" t="s">
+      <c r="P79" s="4" t="s">
         <v>9</v>
       </c>
       <c r="R79" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="5" t="s">
+    <row r="80" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+      <c r="A80" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B80" t="s">
@@ -4683,10 +4731,10 @@
       <c r="D80" t="s">
         <v>279</v>
       </c>
-      <c r="E80" s="14" t="s">
+      <c r="E80" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="F80" s="11">
+      <c r="F80" s="8">
         <v>45014</v>
       </c>
       <c r="I80" t="s">
@@ -4695,13 +4743,13 @@
       <c r="J80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K80" s="5"/>
-      <c r="P80" s="5" t="s">
+      <c r="K80" s="19"/>
+      <c r="P80" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B81" t="s">
@@ -4710,10 +4758,10 @@
       <c r="D81" t="s">
         <v>280</v>
       </c>
-      <c r="E81" s="14" t="s">
+      <c r="E81" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="F81" s="11">
+      <c r="F81" s="8">
         <v>45014</v>
       </c>
       <c r="I81" t="s">
@@ -4722,10 +4770,10 @@
       <c r="J81" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K81" s="5" t="s">
+      <c r="K81" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="P81" s="5" t="s">
+      <c r="P81" s="4" t="s">
         <v>9</v>
       </c>
       <c r="R81" t="s">
@@ -4733,7 +4781,7 @@
       </c>
     </row>
     <row r="82" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B82" t="s">
@@ -4745,7 +4793,7 @@
       <c r="E82" t="s">
         <v>281</v>
       </c>
-      <c r="F82" s="11">
+      <c r="F82" s="8">
         <v>45014</v>
       </c>
       <c r="I82" t="s">
@@ -4754,7 +4802,7 @@
       <c r="J82" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K82" s="5" t="s">
+      <c r="K82" s="19" t="s">
         <v>9</v>
       </c>
       <c r="L82">
@@ -4763,170 +4811,308 @@
       <c r="N82">
         <v>1</v>
       </c>
-      <c r="P82" s="5" t="s">
+      <c r="P82" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q82">
         <v>1</v>
       </c>
-      <c r="R82" s="5" t="s">
+      <c r="R82" s="4" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="19" t="s">
+    <row r="83" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+      <c r="A83" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="C83" s="11">
-        <v>45010</v>
+      <c r="C83" s="8">
+        <v>45070</v>
       </c>
       <c r="D83" t="s">
         <v>311</v>
       </c>
-      <c r="E83" s="17" t="s">
+      <c r="E83" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="F83" s="11">
+      <c r="F83" s="8">
         <v>45009</v>
       </c>
-      <c r="K83" s="5" t="s">
+      <c r="K83" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="P83" s="5" t="s">
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="P83" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="4" t="s">
         <v>305</v>
       </c>
       <c r="B84" t="s">
         <v>317</v>
       </c>
-      <c r="C84" s="11">
-        <v>45010</v>
+      <c r="C84" s="8">
+        <v>45070</v>
       </c>
       <c r="D84" t="s">
         <v>312</v>
       </c>
-      <c r="E84" s="17" t="s">
+      <c r="E84" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="F84" s="11">
+      <c r="F84" s="8">
         <v>45009</v>
       </c>
-      <c r="K84" s="5" t="s">
+      <c r="K84" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P84" s="5" t="s">
+      <c r="L84">
+        <v>1</v>
+      </c>
+      <c r="N84">
+        <v>1</v>
+      </c>
+      <c r="P84" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="4" t="s">
         <v>305</v>
       </c>
       <c r="B85" t="s">
         <v>318</v>
       </c>
-      <c r="C85" s="11">
-        <v>45010</v>
+      <c r="C85" s="8">
+        <v>45070</v>
       </c>
       <c r="D85" t="s">
         <v>313</v>
       </c>
-      <c r="E85" s="17" t="s">
+      <c r="E85" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="F85" s="11">
+      <c r="F85" s="8">
         <v>45009</v>
       </c>
-      <c r="K85" s="5" t="s">
+      <c r="K85" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P85" s="5" t="s">
+      <c r="L85">
+        <v>1</v>
+      </c>
+      <c r="N85">
+        <v>1</v>
+      </c>
+      <c r="P85" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="4" t="s">
         <v>305</v>
       </c>
       <c r="B86" t="s">
         <v>319</v>
       </c>
-      <c r="C86" s="11">
-        <v>45010</v>
+      <c r="C86" s="8">
+        <v>45070</v>
       </c>
       <c r="D86" t="s">
         <v>314</v>
       </c>
-      <c r="E86" s="17" t="s">
+      <c r="E86" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="F86" s="11">
+      <c r="F86" s="8">
         <v>45009</v>
       </c>
-      <c r="K86" s="5" t="s">
+      <c r="K86" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P86" s="5" t="s">
+      <c r="L86">
+        <v>1</v>
+      </c>
+      <c r="N86">
+        <v>1</v>
+      </c>
+      <c r="P86" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="4" t="s">
         <v>305</v>
       </c>
       <c r="B87" t="s">
         <v>320</v>
       </c>
-      <c r="C87" s="11">
-        <v>45010</v>
+      <c r="C87" s="8">
+        <v>45070</v>
       </c>
       <c r="D87" t="s">
         <v>315</v>
       </c>
-      <c r="E87" s="17" t="s">
+      <c r="E87" s="14" t="s">
         <v>310</v>
       </c>
-      <c r="F87" s="11">
+      <c r="F87" s="8">
         <v>45009</v>
       </c>
-      <c r="K87" s="5" t="s">
+      <c r="K87" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P87" s="5" t="s">
-        <v>9</v>
+      <c r="L87">
+        <v>1</v>
+      </c>
+      <c r="N87">
+        <v>1</v>
+      </c>
+      <c r="P87" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R87" s="4" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="5"/>
-      <c r="P88" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A88" s="4"/>
+      <c r="C88" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E88" t="s">
+        <v>323</v>
+      </c>
+      <c r="P88" s="4"/>
     </row>
     <row r="89" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P89" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="C89" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E89" t="s">
+        <v>324</v>
+      </c>
+      <c r="P89" s="4"/>
     </row>
     <row r="90" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P90" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="C90" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E90" t="s">
+        <v>325</v>
+      </c>
+      <c r="P90" s="4"/>
     </row>
     <row r="91" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P91" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="C91" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E91" t="s">
+        <v>326</v>
+      </c>
+      <c r="P91" s="4"/>
     </row>
     <row r="92" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P92" s="5" t="s">
-        <v>9</v>
+      <c r="C92" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E92" t="s">
+        <v>327</v>
+      </c>
+      <c r="P92" s="4"/>
+    </row>
+    <row r="93" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C93" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E93" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C94" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E94" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C95" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E95" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C96" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E96" s="21" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C97" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E97" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="98" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C98" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E98" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="99" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C99" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E99" s="21" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="100" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C100" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E100" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="101" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C101" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E101" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="102" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C102" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E102" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="103" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C103" s="8">
+        <v>45082</v>
+      </c>
+      <c r="E103" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SJG CL 13 participants 662023
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melanieruiz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farerilab/Documents/GitHub/Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82245C38-7AAE-0849-B665-30B47338628C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A2EF13-7EFC-3342-8F96-9E64B62C2828}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="760" windowWidth="16300" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16340" yWindow="2340" windowWidth="25000" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="377">
   <si>
     <t>pavlovia_task</t>
   </si>
@@ -1051,6 +1038,120 @@
   </si>
   <si>
     <t>61002b174a64f106fb46f6a0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flatlined from AQ_14-18, 33-36 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">flatlined from AQ_19-22 and SCS_1-6 </t>
+  </si>
+  <si>
+    <t>R_2WI1ZcAhiPZEWJk</t>
+  </si>
+  <si>
+    <t>R_3oLXnNQXyUAtdUv</t>
+  </si>
+  <si>
+    <t>R_11X96cJ5YkT9Idc</t>
+  </si>
+  <si>
+    <t>R_0MMJik8ROrQwjXb</t>
+  </si>
+  <si>
+    <t>R_2f6sBMR0OkLEFdA</t>
+  </si>
+  <si>
+    <t>R_tQiQ8AV4JwpetMd</t>
+  </si>
+  <si>
+    <t>R_5hcgoIAIrdpRnBD</t>
+  </si>
+  <si>
+    <t>R_3ssjJhOCBMamfWm</t>
+  </si>
+  <si>
+    <t>R_OJp63UmMNzYwIdb</t>
+  </si>
+  <si>
+    <t>R_1mrrlYcOiMZT9sP</t>
+  </si>
+  <si>
+    <t>R_1jTyl83cB4leN0y</t>
+  </si>
+  <si>
+    <t>R_3st7HodBVfKBO1W</t>
+  </si>
+  <si>
+    <t>R_21yUVSiJhXD8Nza</t>
+  </si>
+  <si>
+    <t>R_4YGw381UcVbM29X</t>
+  </si>
+  <si>
+    <t>R_3koGtlT5xjYmjKO</t>
+  </si>
+  <si>
+    <t>R_Y0k1eVb9ztdcMUx</t>
+  </si>
+  <si>
+    <t>R_ywoeZRjCIR22WBP</t>
+  </si>
+  <si>
+    <t>R_2wn7Zst2ZACPSmk</t>
+  </si>
+  <si>
+    <t>R_2rMZ4SeGPrJP1Xb</t>
+  </si>
+  <si>
+    <t>R_1dbi2vWUSGEcMVs</t>
+  </si>
+  <si>
+    <t>R_SUmAxY6kPvEaOQh</t>
+  </si>
+  <si>
+    <t>R_1d5p2oBOYtQfFGi</t>
+  </si>
+  <si>
+    <t>R_2WAzx6bnCoRq9o9</t>
+  </si>
+  <si>
+    <t>R_20PybssV5Z3C9iM</t>
+  </si>
+  <si>
+    <t>R_3CIy28bZBKqzn5G</t>
+  </si>
+  <si>
+    <t>R_5A2i31kzQrTUd69</t>
+  </si>
+  <si>
+    <t>R_1FsHAhu9EXQ5TmS</t>
+  </si>
+  <si>
+    <t>R_2tgIK0jKoSmTvqN</t>
+  </si>
+  <si>
+    <t>R_vVSuE0vXYxESpVv</t>
+  </si>
+  <si>
+    <t>R_3khTEPxyDSF9LLU</t>
+  </si>
+  <si>
+    <t>kept first set of responses</t>
+  </si>
+  <si>
+    <t>changed photo17 w/ photo31 - photos were too similar</t>
+  </si>
+  <si>
+    <t>R_OwZntD3wiJ8Iklr</t>
+  </si>
+  <si>
+    <t>no photos of themselves</t>
+  </si>
+  <si>
+    <t>photo2 repalced w/ photo31</t>
+  </si>
+  <si>
+    <t>no photos</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1178,7 +1279,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1472,10 +1575,10 @@
   <dimension ref="A1:V103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D93" sqref="D93"/>
+      <selection pane="bottomRight" activeCell="C92" sqref="C92:F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1483,15 +1586,19 @@
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="25.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" style="20" hidden="1" customWidth="1"/>
-    <col min="12" max="14" width="25.5" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="25.6640625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="19.83203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="26" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" customWidth="1"/>
+    <col min="15" max="15" width="19.5" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.83203125" customWidth="1"/>
+    <col min="18" max="18" width="103.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1597,7 +1704,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1">
         <f>COUNTA(B2:B998)</f>
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="U2" s="1">
         <f>COUNTIF(S2:S998, "y")</f>
@@ -4822,10 +4929,10 @@
       </c>
     </row>
     <row r="83" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A83" s="16" t="s">
+      <c r="A83" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="22" t="s">
         <v>316</v>
       </c>
       <c r="C83" s="8">
@@ -4834,7 +4941,7 @@
       <c r="D83" t="s">
         <v>311</v>
       </c>
-      <c r="E83" s="14" t="s">
+      <c r="E83" s="22" t="s">
         <v>306</v>
       </c>
       <c r="F83" s="8">
@@ -4863,7 +4970,7 @@
       <c r="D84" t="s">
         <v>312</v>
       </c>
-      <c r="E84" s="14" t="s">
+      <c r="E84" s="22" t="s">
         <v>307</v>
       </c>
       <c r="F84" s="8">
@@ -4895,7 +5002,7 @@
       <c r="D85" t="s">
         <v>313</v>
       </c>
-      <c r="E85" s="14" t="s">
+      <c r="E85" s="22" t="s">
         <v>308</v>
       </c>
       <c r="F85" s="8">
@@ -4927,7 +5034,7 @@
       <c r="D86" t="s">
         <v>314</v>
       </c>
-      <c r="E86" s="14" t="s">
+      <c r="E86" s="22" t="s">
         <v>309</v>
       </c>
       <c r="F86" s="8">
@@ -4959,7 +5066,7 @@
       <c r="D87" t="s">
         <v>315</v>
       </c>
-      <c r="E87" s="14" t="s">
+      <c r="E87" s="22" t="s">
         <v>310</v>
       </c>
       <c r="F87" s="8">
@@ -4982,137 +5089,390 @@
       </c>
     </row>
     <row r="88" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="4"/>
+      <c r="A88" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>357</v>
+      </c>
       <c r="C88" s="8">
         <v>45082</v>
       </c>
-      <c r="E88" t="s">
+      <c r="D88" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="E88" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="P88" s="4"/>
+      <c r="K88" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P88" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R88" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="89" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>358</v>
+      </c>
       <c r="C89" s="8">
         <v>45082</v>
       </c>
-      <c r="E89" t="s">
+      <c r="D89" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="E89" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="P89" s="4"/>
+      <c r="K89" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P89" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R89" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="90" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>359</v>
+      </c>
       <c r="C90" s="8">
         <v>45082</v>
       </c>
-      <c r="E90" t="s">
+      <c r="D90" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="E90" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="P90" s="4"/>
+      <c r="K90" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P90" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="91" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>373</v>
+      </c>
       <c r="C91" s="8">
         <v>45082</v>
       </c>
-      <c r="E91" t="s">
+      <c r="D91" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="E91" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="P91" s="4"/>
+      <c r="K91" t="s">
+        <v>374</v>
+      </c>
+      <c r="P91" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R91" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="92" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>360</v>
+      </c>
       <c r="C92" s="8">
         <v>45082</v>
       </c>
-      <c r="E92" t="s">
+      <c r="D92" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="E92" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="P92" s="4"/>
+      <c r="K92" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P92" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="93" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>361</v>
+      </c>
       <c r="C93" s="8">
         <v>45082</v>
       </c>
-      <c r="E93" t="s">
+      <c r="D93" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="E93" s="14" t="s">
         <v>328</v>
       </c>
+      <c r="K93" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P93" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="94" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>362</v>
+      </c>
       <c r="C94" s="8">
         <v>45082</v>
       </c>
-      <c r="E94" t="s">
+      <c r="D94" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="E94" s="14" t="s">
         <v>329</v>
       </c>
+      <c r="K94" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P94" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R94" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="95" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>363</v>
+      </c>
       <c r="C95" s="8">
         <v>45082</v>
       </c>
-      <c r="E95" t="s">
+      <c r="D95" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="E95" s="14" t="s">
         <v>330</v>
       </c>
+      <c r="K95" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P95" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R95" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="96" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>364</v>
+      </c>
       <c r="C96" s="8">
         <v>45082</v>
       </c>
-      <c r="E96" s="21" t="s">
+      <c r="D96" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="E96" s="23" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="97" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K96" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P96" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>366</v>
+      </c>
       <c r="C97" s="8">
         <v>45082</v>
       </c>
-      <c r="E97" t="s">
+      <c r="D97" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="E97" s="14" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="98" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K97" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P97" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>365</v>
+      </c>
       <c r="C98" s="8">
         <v>45082</v>
       </c>
-      <c r="E98" t="s">
+      <c r="D98" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="E98" s="14" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="99" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K98" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P98" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99" s="14"/>
       <c r="C99" s="8">
         <v>45082</v>
       </c>
-      <c r="E99" s="21" t="s">
+      <c r="D99" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="E99" s="23" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="100" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K99" t="s">
+        <v>376</v>
+      </c>
+      <c r="P99" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>367</v>
+      </c>
       <c r="C100" s="8">
         <v>45082</v>
       </c>
-      <c r="E100" t="s">
+      <c r="D100" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="E100" s="14" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="101" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K100" t="s">
+        <v>374</v>
+      </c>
+      <c r="P100" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R100" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>368</v>
+      </c>
       <c r="C101" s="8">
         <v>45082</v>
       </c>
-      <c r="E101" t="s">
+      <c r="D101" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="E101" s="14" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="102" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K101" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P101" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R101" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>369</v>
+      </c>
       <c r="C102" s="8">
         <v>45082</v>
       </c>
-      <c r="E102" t="s">
+      <c r="D102" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="E102" s="14" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="103" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K102" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P102" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>370</v>
+      </c>
       <c r="C103" s="8">
         <v>45082</v>
       </c>
-      <c r="E103" t="s">
+      <c r="D103" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="E103" s="14" t="s">
         <v>338</v>
+      </c>
+      <c r="K103" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P103" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JD - updated stats and figures
Updated LSAS stats in jnotebook, added sddev in participant list for time between.
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordansiegel/Documents/GitHub/Rejection_Choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CA1025-24B1-5246-85AE-80EEFFAE3F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8258DDA7-858B-8242-ABA2-940D7DDD0C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="16660" windowWidth="24460" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilottotalparticipant_list" sheetId="1" r:id="rId1"/>
@@ -1894,10 +1894,10 @@
   <dimension ref="A1:W133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="180" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="O131" sqref="O131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9343,17 +9343,23 @@
         <v>7.4352941176470591</v>
       </c>
     </row>
-    <row r="131" spans="19:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="15:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O130">
+        <f>STDEV(O125,O123,O120:O121,O117:O118,O114:O115,O109:O112,O106,O103:O104,O100,O98,O87:O92,O83:O84,O78:O80,O76,O70,O70,O67:O68,O59:O65,O34:O55,O31:O32,O27:O28,O24:O25,O17:O21,O13:O15,O2:O10)</f>
+        <v>11.266730478993207</v>
+      </c>
+    </row>
+    <row r="131" spans="15:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="S131" s="4">
         <v>27</v>
       </c>
     </row>
-    <row r="132" spans="19:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="15:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="S132">
         <v>56</v>
       </c>
     </row>
-    <row r="133" spans="19:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="15:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="S133">
         <v>1</v>
       </c>

</xml_diff>